<commit_message>
Working on the vignette
</commit_message>
<xml_diff>
--- a/inst/extdata/example-criteria-weights.xlsx
+++ b/inst/extdata/example-criteria-weights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Data\R\dmcda\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBF296A-A7BA-4A55-B0EF-B2F3527838B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6082F0F6-8F8E-4A7D-84E2-8D4906A39EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="46">
   <si>
     <t>scorer</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>outcomes</t>
   </si>
   <si>
     <t>crime</t>
@@ -451,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z973"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -478,25 +475,25 @@
         <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>1</v>
@@ -520,31 +517,31 @@
     </row>
     <row r="2" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>6</v>
@@ -568,34 +565,34 @@
     </row>
     <row r="3" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -616,34 +613,34 @@
     </row>
     <row r="4" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="4">
         <v>-100</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="4">
         <v>100</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -664,34 +661,34 @@
     </row>
     <row r="5" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4">
         <v>-100</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="4">
         <v>100</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -712,34 +709,34 @@
     </row>
     <row r="6" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -760,34 +757,34 @@
     </row>
     <row r="7" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="4">
         <v>-100</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="4">
         <v>100</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -808,34 +805,34 @@
     </row>
     <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4">
         <v>-100</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="4">
         <v>100</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -856,34 +853,34 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -904,34 +901,34 @@
     </row>
     <row r="10" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="4">
         <v>-100</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="4">
         <v>0</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="4">
         <v>100</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -952,34 +949,34 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="4">
         <v>-100</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="4">
         <v>100</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -27983,13 +27980,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -27997,16 +27994,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3">
         <v>40</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -28014,16 +28011,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3">
         <v>30</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -28031,16 +28028,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -28048,16 +28045,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <v>100</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -28065,16 +28062,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3">
         <v>100</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -28082,16 +28079,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>80</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -28099,16 +28096,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3">
         <v>60</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -28116,16 +28113,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3">
         <v>100</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -28133,16 +28130,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3">
         <v>40</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29152,172 +29149,172 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3">
         <v>80</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3">
         <v>100</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>70</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3">
         <v>70</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>100</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3">
         <v>100</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3">
         <v>80</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3">
         <v>100</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30294,7 +30291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E975"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -30327,172 +30324,172 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3">
         <v>80</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3">
         <v>70</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3">
         <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <v>100</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3">
         <v>100</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3">
         <v>70</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3">
         <v>100</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3">
         <v>60</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>